<commit_message>
fix: problem with bulk register
</commit_message>
<xml_diff>
--- a/Excel/Users.xlsx
+++ b/Excel/Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\proyecto\PlanAcadProject\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E50CCA-3281-4869-89B7-FDBCCA575A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE2A0AD-0989-4CA7-A6AF-AFBB81096E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>first_name</t>
   </si>
@@ -52,13 +52,16 @@
   </si>
   <si>
     <t>IQ</t>
+  </si>
+  <si>
+    <t>legajo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +79,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,12 +113,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -389,55 +401,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>23001</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4113609</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{59BBAA36-A35A-42F1-A9F3-6E88299801F5}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{59BBAA36-A35A-42F1-A9F3-6E88299801F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>